<commit_message>
Worked on references and word editing
</commit_message>
<xml_diff>
--- a/Results/Tables/Asthma_result.xlsx
+++ b/Results/Tables/Asthma_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9255" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2006_count" sheetId="1" r:id="rId1"/>
@@ -4522,7 +4522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
@@ -10274,7 +10274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>

</xml_diff>